<commit_message>
Fix data type detection, add test for failed batch download
</commit_message>
<xml_diff>
--- a/Excel-4.xlsx
+++ b/Excel-4.xlsx
@@ -43,34 +43,34 @@
     <t>A</t>
   </si>
   <si>
+    <t>s-006</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Class-C</t>
+  </si>
+  <si>
+    <t>s-011</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>s-001</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
     <t>s-003</t>
   </si>
   <si>
     <t>Jennifer</t>
-  </si>
-  <si>
-    <t>s-006</t>
-  </si>
-  <si>
-    <t>Susan</t>
-  </si>
-  <si>
-    <t>Class-C</t>
-  </si>
-  <si>
-    <t>s-011</t>
-  </si>
-  <si>
-    <t>Charles</t>
-  </si>
-  <si>
-    <t>s-001</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>A+</t>
   </si>
   <si>
     <t>s-007</t>
@@ -194,7 +194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -242,7 +242,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>7</v>
@@ -250,29 +250,15 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>12</v>
-      </c>
       <c r="D4" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s" s="2">
         <v>7</v>
       </c>
     </row>
@@ -283,7 +269,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -311,30 +297,44 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>6</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B4" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="C3" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>17</v>
+      <c r="C4" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>